<commit_message>
create backup before making branch with gsap timeline
</commit_message>
<xml_diff>
--- a/Changes.xlsx
+++ b/Changes.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="autoNext" sheetId="1" r:id="rId1"/>
-    <sheet name="playNewMedia" sheetId="2" r:id="rId2"/>
+    <sheet name="behavior" sheetId="2" r:id="rId2"/>
     <sheet name="mediaClass constructor" sheetId="3" r:id="rId3"/>
     <sheet name="play" sheetId="4" r:id="rId4"/>
     <sheet name="nextprev" sheetId="5" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>function</t>
   </si>
@@ -284,6 +284,136 @@
   </si>
   <si>
     <t>tag and filename OK</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>resume</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>animations</t>
+  </si>
+  <si>
+    <t>backgrounds (no transition)</t>
+  </si>
+  <si>
+    <t>audio - narration</t>
+  </si>
+  <si>
+    <t>audio - background</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause and leave settings
+no changes to timeline which is stopped
+</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>play from currentTime</t>
+  </si>
+  <si>
+    <t>pause and keep currentTime</t>
+  </si>
+  <si>
+    <t>pause and set currentTime to offsetTime</t>
+  </si>
+  <si>
+    <t>audio narration</t>
+  </si>
+  <si>
+    <t>initialize media (new slide)</t>
+  </si>
+  <si>
+    <t>if duration &lt; 0, set class to keep
+if delay &lt; 0, set class to no preload
+add json settings to mediaClass.
+Connect audio to it’s gain stage but do not connect gain to masterVolume</t>
+  </si>
+  <si>
+    <t>if (delay &gt; =0)
+    play from currentTime after delay
+if delay &lt;0 play from currentTIme</t>
+  </si>
+  <si>
+    <t>stop timers
+stop all unfinished slides and animations.
+Tranout - tran then remove elements that do not have class = "keep"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop playing current
+load next 
+    if (next = current)
+</t>
+  </si>
+  <si>
+    <t>we don't really have the ability to determine next or prev source.
+if (next src is same as current src)
+     if (offsetTime &gt; 0)
+              set curretTIme to offsetTime</t>
+  </si>
+  <si>
+    <t>duration and delay can be negative if the background crosses two slides
+default volume is 0.4</t>
+  </si>
+  <si>
+    <t>duration and delay can be negative if the narration crosses two slides
+default volume is 0.9</t>
+  </si>
+  <si>
+    <t>duration and delay should not be negative because we likely do not want video crossing slides
+default volume is 0.9
+consider shutting off or at least decreasing background volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">play from wherever it is
+should I consume settings?
+Settings should already be defined and set including volume level.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause elements that do not have keep set
+</t>
+  </si>
+  <si>
+    <t>stop playing (Same as stop)
+back to prev slide
+initialize media
+consume settings for that slide
+set things up so that when play hits, it can just play</t>
+  </si>
+  <si>
+    <t>stop playing (Same as stop)
+advance to next slide
+initialize media
+consume settings for that slide
+set things up so that when play hits, it can just play</t>
+  </si>
+  <si>
+    <t>pause and reset to 0 or offsetTime
+slide number does not change.
+Whatever slide we are on, set the levels, etc to that slide
+disconnect gain node</t>
   </si>
 </sst>
 </file>
@@ -332,13 +462,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C35"/>
+  <dimension ref="A3:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>33</v>
       </c>
@@ -796,7 +929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>34</v>
       </c>
@@ -804,12 +937,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -820,12 +958,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="D4" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:B4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -834,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
backup incase I scrw something up. Rewritng so I can use json data
</commit_message>
<xml_diff>
--- a/Changes.xlsx
+++ b/Changes.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="4590" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="autoNext" sheetId="1" r:id="rId1"/>
-    <sheet name="behavior" sheetId="2" r:id="rId2"/>
-    <sheet name="mediaClass constructor" sheetId="3" r:id="rId3"/>
-    <sheet name="play" sheetId="4" r:id="rId4"/>
-    <sheet name="nextprev" sheetId="5" r:id="rId5"/>
-    <sheet name="volume" sheetId="6" r:id="rId6"/>
+    <sheet name="behavior with gSap" sheetId="7" r:id="rId1"/>
+    <sheet name="mediaclass" sheetId="8" r:id="rId2"/>
+    <sheet name="behavior" sheetId="2" r:id="rId3"/>
+    <sheet name="autoNext" sheetId="1" r:id="rId4"/>
+    <sheet name="mediaClass constructor" sheetId="3" r:id="rId5"/>
+    <sheet name="play" sheetId="4" r:id="rId6"/>
+    <sheet name="nextprev" sheetId="5" r:id="rId7"/>
+    <sheet name="volume" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="174">
   <si>
     <t>function</t>
   </si>
@@ -299,6 +301,9 @@
   </si>
   <si>
     <t>resume</t>
+  </si>
+  <si>
+    <t>audio</t>
   </si>
   <si>
     <t>video</t>
@@ -389,10 +394,6 @@
     <t xml:space="preserve">play from wherever it is
 should I consume settings?
 Settings should already be defined and set including volume level.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pause elements that do not have keep set
 </t>
   </si>
   <si>
@@ -414,6 +415,187 @@
 slide number does not change.
 Whatever slide we are on, set the levels, etc to that slide
 disconnect gain node</t>
+  </si>
+  <si>
+    <t>pause elements that do not have keep set
+gainNode goes with the media array.
+So if class = keep, just let it ride
+if class != keep, leave it as current.
+Update the audiCtx to match dataset</t>
+  </si>
+  <si>
+    <t>Set up all tweens</t>
+  </si>
+  <si>
+    <t>master timeline keeps track of slides</t>
+  </si>
+  <si>
+    <t>slide timeline keeps track of media within a slide</t>
+  </si>
+  <si>
+    <t>A slide is a tween for the presentation</t>
+  </si>
+  <si>
+    <t>Do not load source until ready for tween</t>
+  </si>
+  <si>
+    <t>Each slide tween knows who is next and previous?</t>
+  </si>
+  <si>
+    <t>play from where the timeline is</t>
+  </si>
+  <si>
+    <t>Splash screen is first slide (slide 0)</t>
+  </si>
+  <si>
+    <t>rewind</t>
+  </si>
+  <si>
+    <t>set to either splash or to slide 1 depending on setting</t>
+  </si>
+  <si>
+    <t>timeline</t>
+  </si>
+  <si>
+    <t>slide timeline</t>
+  </si>
+  <si>
+    <t>each media is a tween</t>
+  </si>
+  <si>
+    <t>each tween has a delay, a target, a duration and an effect, and an offset</t>
+  </si>
+  <si>
+    <t>mapping json to tween: target = DOM element except audio</t>
+  </si>
+  <si>
+    <t>if (delay &gt; 0) just set  delay</t>
+  </si>
+  <si>
+    <t>if (delay &lt; 0) I think we just ignore it</t>
+  </si>
+  <si>
+    <t>let the tween just finish and die when tranout occurs</t>
+  </si>
+  <si>
+    <t>slide time 0 is when previous slide starts tranout</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>the element to target</t>
+  </si>
+  <si>
+    <t>base class - animation &amp; transition</t>
+  </si>
+  <si>
+    <t>ptr to the next slide</t>
+  </si>
+  <si>
+    <t>ptr to the prev slide</t>
+  </si>
+  <si>
+    <t>the timeline for the slide
+animations and other media get added</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>the slide name or label to help find the timeline</t>
+  </si>
+  <si>
+    <t>img class</t>
+  </si>
+  <si>
+    <t>json attributes</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>transition</t>
+  </si>
+  <si>
+    <t>trancss or from - array of effects</t>
+  </si>
+  <si>
+    <t>animations?</t>
+  </si>
+  <si>
+    <t>slideTitle</t>
+  </si>
+  <si>
+    <t>slideNo (change to slide name)</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>classLst</t>
+  </si>
+  <si>
+    <t>source/text</t>
+  </si>
+  <si>
+    <t>offsetTime</t>
+  </si>
+  <si>
+    <t>tranIn - array of effects</t>
+  </si>
+  <si>
+    <t>tranOut - array of effects</t>
+  </si>
+  <si>
+    <t>transition pattern</t>
+  </si>
+  <si>
+    <t>trancss/from: is where it starts, 
+duration, scaleX, opacity, etc</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>innerHTML</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>maybe?</t>
+  </si>
+  <si>
+    <t>ht4f_audio,
+[background],
+[narration]</t>
+  </si>
+  <si>
+    <t>ht4f_video</t>
+  </si>
+  <si>
+    <t>ht4f_image, 
+ht4f_aspect,
+[animation]</t>
+  </si>
+  <si>
+    <t>[animation]</t>
   </si>
 </sst>
 </file>
@@ -436,7 +618,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,6 +628,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -471,6 +659,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,6 +682,1731 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8458199" y="161925"/>
+          <a:ext cx="6105525" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>master</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> timeline</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>154555</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>526783</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>64708</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>183171</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="Group 19"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11606536" y="1479283"/>
+          <a:ext cx="2950826" cy="1561388"/>
+          <a:chOff x="8609824" y="753918"/>
+          <a:chExt cx="2950826" cy="799388"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9190469" y="754812"/>
+            <a:ext cx="1640113" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>slide timeline</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8609824" y="756069"/>
+            <a:ext cx="731520" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>tran-In</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rectangle 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10829130" y="753918"/>
+            <a:ext cx="731520" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>tran-out</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9532882" y="1126473"/>
+            <a:ext cx="1007796" cy="214216"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+              <a:alpha val="28000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>anim</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> tween</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+          <xdr:cNvCxnSpPr>
+            <a:endCxn id="8" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9317221" y="1229264"/>
+            <a:ext cx="215661" cy="4317"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="Straight Connector 12"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9328419" y="1164566"/>
+            <a:ext cx="3594" cy="291142"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="14" name="Straight Arrow Connector 13"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="17" idx="1"/>
+            <a:endCxn id="17" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9515049" y="1465240"/>
+            <a:ext cx="1029363" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="TextBox 16"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9515049" y="1377174"/>
+            <a:ext cx="1029363" cy="176132"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="39000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>duration</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556070</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180952</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>466223</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>49821</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="Group 20"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13832455" y="2466952"/>
+          <a:ext cx="2950826" cy="1011869"/>
+          <a:chOff x="8609824" y="753918"/>
+          <a:chExt cx="2950826" cy="821369"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="Rectangle 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9190469" y="754812"/>
+            <a:ext cx="1640113" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>slide timeline</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Rectangle 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8609824" y="756069"/>
+            <a:ext cx="731520" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>tran-In</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="Rectangle 23"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10829130" y="753918"/>
+            <a:ext cx="731520" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>tran-out</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="Rectangle 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9606152" y="1126473"/>
+            <a:ext cx="1007796" cy="214216"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+              <a:alpha val="28000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>anim</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> tween</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
+          <xdr:cNvCxnSpPr>
+            <a:endCxn id="25" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9343293" y="1225062"/>
+            <a:ext cx="262859" cy="8519"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="27" name="Straight Connector 26"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9335746" y="1164566"/>
+            <a:ext cx="3594" cy="291142"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="29" idx="1"/>
+            <a:endCxn id="29" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9588319" y="1487221"/>
+            <a:ext cx="1029363" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="TextBox 28"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9588319" y="1399155"/>
+            <a:ext cx="1029363" cy="176132"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:alpha val="39000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>duration</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>153866</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>153865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>21980</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10484828" y="3582865"/>
+          <a:ext cx="5605095" cy="249115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Background audio</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>131885</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>131884</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556846</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10462847" y="3941884"/>
+          <a:ext cx="424961" cy="205154"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>512884</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>263769</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80597</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11451980" y="4066442"/>
+          <a:ext cx="967154" cy="14655"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>249115</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600808</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12404480" y="3971192"/>
+          <a:ext cx="351693" cy="95251"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>578827</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>73270</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12734192" y="3978519"/>
+          <a:ext cx="710713" cy="7327"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>307731</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168518</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>439616</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168519</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14895635" y="3978518"/>
+          <a:ext cx="740019" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>254977</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>130419</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>512884</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80596</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11194073" y="3940419"/>
+          <a:ext cx="257907" cy="140677"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556846</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>131884</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>278423</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139211</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Connector 54"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10887808" y="3941884"/>
+          <a:ext cx="329711" cy="7327"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>36635</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13408270" y="3978519"/>
+          <a:ext cx="249115" cy="109904"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276958</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>86457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>109903</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Connector 56"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13648593" y="4086957"/>
+          <a:ext cx="1049214" cy="1466"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>93784</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>344365</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>86457</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Connector 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14681688" y="3971192"/>
+          <a:ext cx="250581" cy="115765"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>564173</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>73269</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5271700" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="TextBox 79"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10895135" y="4264269"/>
+          <a:ext cx="5271700" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>background volume level when auto-level is enabled. It auto drops when narration starts</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>48387</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>105477</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="463910"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="TextBox 80"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17409777">
+          <a:off x="10279674" y="1157652"/>
+          <a:ext cx="463910" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>from</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14653</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>271096</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>435882</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>615122</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="TextBox 82"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10345615" y="1223596"/>
+          <a:ext cx="1029363" cy="344026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>duration</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>197827</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>254652</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="306302"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="TextBox 83"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17409777">
+          <a:off x="11116052" y="1228023"/>
+          <a:ext cx="306302" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>to</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>461596</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>247324</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="306302"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="TextBox 84"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17409777">
+          <a:off x="12596090" y="1220695"/>
+          <a:ext cx="306302" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>to</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556846</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>234461</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="306302"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="TextBox 85"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17409777">
+          <a:off x="13299475" y="1207832"/>
+          <a:ext cx="306302" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>to</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -752,216 +2672,474 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C39"/>
+  <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
       <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" t="s">
+        <v>169</v>
+      </c>
+      <c r="I13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" t="s">
+        <v>171</v>
+      </c>
+      <c r="H15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,50 +3159,50 @@
         <v>85</v>
       </c>
       <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
         <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1032,10 +3210,10 @@
         <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1043,10 +3221,10 @@
         <v>87</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1057,7 +3235,7 @@
         <v>116</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1065,34 +3243,34 @@
         <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>114</v>
@@ -1106,7 +3284,213 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
@@ -1319,7 +3703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1331,7 +3715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1343,7 +3727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>

</xml_diff>